<commit_message>
adding vendor feature is done!
adding new vendors to the existing vendor sheet.
</commit_message>
<xml_diff>
--- a/Vendors.xlsx
+++ b/Vendors.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\revature\hbksilver-code\RPA\P0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\revature\hbksilver-code\RPA\P0\P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D197CD01-5CC4-415E-9A77-5C14EB989466}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC1BE15A-B0FA-4F15-B416-EAEC7D6DC38F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2543" yWindow="2543" windowWidth="14400" windowHeight="8272" xr2:uid="{82A886E4-3165-4763-9A20-41C9FA8D299D}"/>
+    <workbookView xWindow="698" yWindow="3098" windowWidth="14400" windowHeight="8272" xr2:uid="{82A886E4-3165-4763-9A20-41C9FA8D299D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">Vendor </t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>www.walmart.com</t>
+  </si>
+  <si>
+    <t>www.netflix.com</t>
+  </si>
+  <si>
+    <t>Netflix</t>
   </si>
 </sst>
 </file>
@@ -432,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02A2116C-CC24-4D89-8E1A-2BEB37DADC95}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -488,6 +494,14 @@
         <v>11</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{51FBDDB6-E697-4B8D-988E-C7675CDB5717}"/>
@@ -495,6 +509,7 @@
     <hyperlink ref="B4" r:id="rId3" xr:uid="{E0D7948B-F769-4EC4-885B-FC09F8A8DFB2}"/>
     <hyperlink ref="B5" r:id="rId4" xr:uid="{E0B59CB3-83B9-4FDA-A409-EF519A01CA49}"/>
     <hyperlink ref="B6" r:id="rId5" xr:uid="{21564785-48F2-4B74-A029-F3203849E978}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{EDFFE1A1-782D-40C6-88D8-6606289F7A19}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Changed the columns in vendor sheet
</commit_message>
<xml_diff>
--- a/Vendors.xlsx
+++ b/Vendors.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\revature\hbksilver-code\RPA\P0\P0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\donation\Desktop\Baraka_H-andAlfaro_G-P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F45B2CB8-4F8B-46D9-85AE-D3DC6F63D4C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E053DC63-78A0-42FA-A5BF-6EF658D46E23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" xr2:uid="{82A886E4-3165-4763-9A20-41C9FA8D299D}"/>
+    <workbookView xWindow="1305" yWindow="-120" windowWidth="27615" windowHeight="16440" xr2:uid="{82A886E4-3165-4763-9A20-41C9FA8D299D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
   <si>
     <t xml:space="preserve">Vendor </t>
   </si>
@@ -140,6 +140,30 @@
   </si>
   <si>
     <t>Original Price</t>
+  </si>
+  <si>
+    <t>ItemName1</t>
+  </si>
+  <si>
+    <t>Price1</t>
+  </si>
+  <si>
+    <t>Discout3</t>
+  </si>
+  <si>
+    <t>FinalPrice3</t>
+  </si>
+  <si>
+    <t>Final Price2</t>
+  </si>
+  <si>
+    <t>Discount2</t>
+  </si>
+  <si>
+    <t>Discount1</t>
+  </si>
+  <si>
+    <t>Final Price1</t>
   </si>
 </sst>
 </file>
@@ -570,30 +594,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02A2116C-CC24-4D89-8E1A-2BEB37DADC95}">
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:U7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.73046875" customWidth="1"/>
-    <col min="2" max="2" width="37.796875" customWidth="1"/>
-    <col min="3" max="3" width="9.06640625" style="3"/>
-    <col min="4" max="4" width="13.46484375" style="6" customWidth="1"/>
-    <col min="6" max="6" width="11.1328125" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.06640625" style="4"/>
-    <col min="8" max="8" width="10.33203125" customWidth="1"/>
-    <col min="9" max="9" width="9.06640625" style="5"/>
-    <col min="12" max="12" width="9.06640625" style="4"/>
-    <col min="13" max="13" width="10.33203125" customWidth="1"/>
-    <col min="14" max="14" width="9.06640625" style="5"/>
-    <col min="16" max="16" width="13.86328125" customWidth="1"/>
-    <col min="17" max="17" width="9.06640625" style="4"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="37.85546875" customWidth="1"/>
+    <col min="3" max="3" width="9" style="3"/>
+    <col min="4" max="4" width="13.42578125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" style="4"/>
+    <col min="8" max="8" width="10.28515625" customWidth="1"/>
+    <col min="9" max="9" width="9" style="5"/>
+    <col min="12" max="12" width="9" style="4"/>
+    <col min="13" max="13" width="10.28515625" customWidth="1"/>
+    <col min="14" max="14" width="9" style="5"/>
+    <col min="16" max="16" width="13.85546875" customWidth="1"/>
+    <col min="17" max="17" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -616,37 +640,49 @@
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="J1" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="K1" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="M1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="O1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="P1" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="Q1" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="R1" t="s">
+        <v>31</v>
+      </c>
+      <c r="S1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T1" t="s">
+        <v>37</v>
+      </c>
+      <c r="U1" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -696,7 +732,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -746,7 +782,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -796,7 +832,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15.4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -846,10 +882,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C7" s="2"/>
     </row>
   </sheetData>
@@ -866,20 +902,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE021577-FBF3-4041-9507-118CDDC93DC0}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="30.3984375" customWidth="1"/>
-    <col min="4" max="4" width="12.3984375" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -890,22 +926,28 @@
         <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added excel sheets and worked on adding expense
</commit_message>
<xml_diff>
--- a/Vendors.xlsx
+++ b/Vendors.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\donation\Desktop\Baraka_H-andAlfaro_G-P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B57521F0-35AC-47BD-8B60-5282736EA40F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEA827C6-1203-40F5-9FF8-300EB1CDD384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10995" yWindow="3240" windowWidth="14565" windowHeight="8310" xr2:uid="{82A886E4-3165-4763-9A20-41C9FA8D299D}"/>
+    <workbookView xWindow="7665" yWindow="3060" windowWidth="14565" windowHeight="8310" xr2:uid="{82A886E4-3165-4763-9A20-41C9FA8D299D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Amazon" sheetId="1" r:id="rId1"/>
-    <sheet name="Walmart" sheetId="2" r:id="rId2"/>
-    <sheet name="Target" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
+    <sheet name="Amazon" sheetId="1" r:id="rId2"/>
+    <sheet name="Walmart" sheetId="2" r:id="rId3"/>
+    <sheet name="Target" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -470,10 +471,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CED089A9-0581-456A-89BE-20FC90845F25}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02A2116C-CC24-4D89-8E1A-2BEB37DADC95}">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -591,7 +606,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F90A4268-83BB-4301-A437-8A99F64E16FD}">
   <dimension ref="A1:L2"/>
   <sheetViews>
@@ -682,7 +697,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EBB4556-605C-42A1-AA94-AF1977A4A82E}">
   <dimension ref="A1:L2"/>
   <sheetViews>

</xml_diff>